<commit_message>
Added remaining contents; Added Colorcoding; Added Freeze pane for top row
</commit_message>
<xml_diff>
--- a/templates/visitExcel.xlsx
+++ b/templates/visitExcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -177,7 +177,13 @@
     <t>Bauphasen</t>
   </si>
   <si>
-    <t>blub</t>
+    <t>Beginn der Bauphase</t>
+  </si>
+  <si>
+    <t>Ende der Bauphase</t>
+  </si>
+  <si>
+    <t>Jahrhundert</t>
   </si>
   <si>
     <t>Enthaltene Bauteile</t>
@@ -268,6 +274,207 @@
   </si>
   <si>
     <t>Verweis auf Ort</t>
+  </si>
+  <si>
+    <t>Objektbezeichnung</t>
+  </si>
+  <si>
+    <t>Allgemeine Objektdatierung</t>
+  </si>
+  <si>
+    <t>Objekt besteht aus Teilobjekten</t>
+  </si>
+  <si>
+    <t>Teilobjekt von</t>
+  </si>
+  <si>
+    <t>Herstellung</t>
+  </si>
+  <si>
+    <t>Künstler</t>
+  </si>
+  <si>
+    <t>Entstehungszeit: Freie Datierung</t>
+  </si>
+  <si>
+    <t>Entstehungszeit: Beginn des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Entstehungszeit: Ende des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Entstehungszeit: Jahrhundert</t>
+  </si>
+  <si>
+    <t>Herstellungsort</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Technik</t>
+  </si>
+  <si>
+    <t>Masse</t>
+  </si>
+  <si>
+    <t>Abmessung</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>Inschrift</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Anbringung</t>
+  </si>
+  <si>
+    <t>Signatur</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Institution/Eigentümer/Verwalter</t>
+  </si>
+  <si>
+    <t>Inventarnummer</t>
+  </si>
+  <si>
+    <t>Standort - Museum</t>
+  </si>
+  <si>
+    <t>Standort - Bauwerk</t>
+  </si>
+  <si>
+    <t>Provenienz</t>
+  </si>
+  <si>
+    <t>Datierung des Besitzerwechsels</t>
+  </si>
+  <si>
+    <t>Eigentümer - Person</t>
+  </si>
+  <si>
+    <t>Eigentümer - Gruppe</t>
+  </si>
+  <si>
+    <t>Vorbesitzer - Person</t>
+  </si>
+  <si>
+    <t>Vorbesitzer - Gruppe</t>
+  </si>
+  <si>
+    <t>Objektbezug</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Abgebildetes Bauwerk</t>
+  </si>
+  <si>
+    <t>Abgebildeter Ort</t>
+  </si>
+  <si>
+    <t>Abgebildete Aktivität</t>
+  </si>
+  <si>
+    <t>Bauwerk</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>Ausstellung</t>
+  </si>
+  <si>
+    <t>Katalog</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Künstlername</t>
+  </si>
+  <si>
+    <t>Notname</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Geburt</t>
+  </si>
+  <si>
+    <t>Geburtsdatum</t>
+  </si>
+  <si>
+    <t>Geburtsort</t>
+  </si>
+  <si>
+    <t>Mutter</t>
+  </si>
+  <si>
+    <t>Vater</t>
+  </si>
+  <si>
+    <t>Tod</t>
+  </si>
+  <si>
+    <t>Sterbedatum</t>
+  </si>
+  <si>
+    <t>Sterbeort</t>
+  </si>
+  <si>
+    <t>Amt/Beruf</t>
+  </si>
+  <si>
+    <t>Ehe</t>
+  </si>
+  <si>
+    <t>Ehepartner</t>
+  </si>
+  <si>
+    <t>Beginn der Ehe</t>
+  </si>
+  <si>
+    <t>Ende der Ehe</t>
+  </si>
+  <si>
+    <t>Kinder</t>
+  </si>
+  <si>
+    <t>Verwaltung/Eigentum</t>
+  </si>
+  <si>
+    <t>Teilnahme</t>
+  </si>
+  <si>
+    <t>Beteiligt an - Bauwerke</t>
+  </si>
+  <si>
+    <t>Beteiligt an - Baumaßnahmen</t>
+  </si>
+  <si>
+    <t>Ortsname</t>
+  </si>
+  <si>
+    <t>Geburtsort von Personen</t>
+  </si>
+  <si>
+    <t>Sterbeort von Personen</t>
+  </si>
+  <si>
+    <t>Abbildung</t>
   </si>
 </sst>
 </file>
@@ -275,7 +482,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="38">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -323,8 +530,153 @@
       <sz val="11.0"/>
       <b val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,8 +703,28 @@
         <fgColor indexed="22"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -361,47 +733,232 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom style="thin"/>
     </border>
     <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
       <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="dashed"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="dashed"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="5" xfId="0" applyFill="true" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -411,8 +968,8 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
@@ -440,23 +997,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" s="3" customFormat="true">
+      <c r="A5" t="s" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="6" s="4" customFormat="true">
+      <c r="A6" t="s" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="7" s="5" customFormat="true">
+      <c r="A7" t="s" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="true">
-      <c r="A8" t="s" s="3">
+    <row r="8" s="7" customFormat="true">
+      <c r="A8" t="s" s="7">
         <v>7</v>
       </c>
     </row>
@@ -490,18 +1047,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" s="4" customFormat="true">
-      <c r="A15" t="s" s="4">
+    <row r="15" s="8" customFormat="true">
+      <c r="A15" t="s" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="16" s="9" customFormat="true">
+      <c r="A16" t="s" s="9">
         <v>15</v>
       </c>
     </row>
-    <row r="17" s="5" customFormat="true">
-      <c r="A17" t="s" s="5">
+    <row r="17" s="11" customFormat="true">
+      <c r="A17" t="s" s="11">
         <v>16</v>
       </c>
     </row>
@@ -511,18 +1068,21 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" sqref="B9:F9" allowBlank="true" errorStyle="stop">
+  <dataValidations count="5">
+    <dataValidation type="list" sqref="B9:SG9" allowBlank="true" errorStyle="stop">
       <formula1>Place!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B10:F10" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B10:SG10" allowBlank="true" errorStyle="stop">
       <formula1>Person!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B11:F11" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B11:SG11" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B12:F12" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B12:SG12" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B16:SG16" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -534,8 +1094,8 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
@@ -543,8 +1103,8 @@
     <col min="1" max="1" width="35.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true">
-      <c r="A1" t="s" s="6">
+    <row r="1" s="12" customFormat="true">
+      <c r="A1" t="s" s="12">
         <v>0</v>
       </c>
     </row>
@@ -608,43 +1168,46 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" s="7" customFormat="true">
-      <c r="A14" t="s" s="7">
+    <row r="14" s="13" customFormat="true">
+      <c r="A14" t="s" s="13">
         <v>14</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="15" s="14" customFormat="true">
+      <c r="A15" t="s" s="14">
         <v>15</v>
       </c>
     </row>
-    <row r="16" s="8" customFormat="true">
-      <c r="A16" t="s" s="8">
+    <row r="16" s="16" customFormat="true">
+      <c r="A16" t="s" s="16">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" sqref="B3:F3" allowBlank="true" errorStyle="stop">
+  <dataValidations count="8">
+    <dataValidation type="list" sqref="B3:SG3" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B4:F4" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B4:SG4" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B5:F5" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B5:SG5" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B6:F6" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B6:SG6" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B7:F7" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B7:SG7" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B11:F11" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B11:SG11" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B12:F12" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B12:SG12" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B15:SG15" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -653,11 +1216,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
@@ -665,8 +1228,8 @@
     <col min="1" max="1" width="40.5546875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true">
-      <c r="A1" t="s" s="9">
+    <row r="1" s="17" customFormat="true">
+      <c r="A1" t="s" s="17">
         <v>0</v>
       </c>
     </row>
@@ -735,168 +1298,277 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" s="10" customFormat="true">
-      <c r="A15" t="s" s="10">
+    <row r="15" s="18" customFormat="true">
+      <c r="A15" t="s" s="18">
         <v>41</v>
       </c>
     </row>
-    <row r="16" s="11" customFormat="true">
-      <c r="A16" t="s" s="11">
+    <row r="16" s="20" customFormat="true">
+      <c r="A16" t="s" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="17" s="21" customFormat="true">
+      <c r="A17" t="s" s="21">
         <v>42</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="18" s="22" customFormat="true">
+      <c r="A18" t="s" s="22">
         <v>43</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="19" s="23" customFormat="true">
+      <c r="A19" t="s" s="23">
         <v>44</v>
       </c>
     </row>
-    <row r="20" s="12" customFormat="true">
-      <c r="A20" t="s" s="12">
+    <row r="20" s="25" customFormat="true">
+      <c r="A20" t="s" s="25">
         <v>45</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="21" s="26" customFormat="true">
+      <c r="A21" t="s" s="26">
         <v>46</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="22" s="27" customFormat="true">
+      <c r="A22" t="s" s="27">
         <v>47</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="23" s="28" customFormat="true">
+      <c r="A23" t="s" s="28">
         <v>9</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="24" s="29" customFormat="true">
+      <c r="A24" t="s" s="29">
         <v>48</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="25" s="30" customFormat="true">
+      <c r="A25" t="s" s="30">
         <v>49</v>
       </c>
     </row>
-    <row r="26" s="13" customFormat="true">
-      <c r="A26" t="s" s="13">
+    <row r="26" s="32" customFormat="true">
+      <c r="A26" t="s" s="32">
         <v>50</v>
       </c>
     </row>
-    <row r="27" s="14" customFormat="true">
-      <c r="A27" t="s" s="14">
+    <row r="27" s="33" customFormat="true">
+      <c r="A27" t="s" s="33">
         <v>51</v>
       </c>
     </row>
-    <row r="28" s="15" customFormat="true">
-      <c r="A28" t="s" s="15">
+    <row r="28" s="34" customFormat="true">
+      <c r="A28" t="s" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" s="36" customFormat="true">
+      <c r="A29" t="s" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" s="37" customFormat="true">
+      <c r="A30" t="s" s="37">
         <v>52</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
+    <row r="31" s="38" customFormat="true">
+      <c r="A31" t="s" s="38">
         <v>53</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
+    <row r="32" s="39" customFormat="true">
+      <c r="A32" t="s" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" s="41" customFormat="true">
+      <c r="A33" t="s" s="41">
         <v>54</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s">
+    <row r="34" s="42" customFormat="true">
+      <c r="A34" t="s" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" s="43" customFormat="true">
+      <c r="A35" t="s" s="43">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" s="44" customFormat="true">
+      <c r="A36" t="s" s="44">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" s="45" customFormat="true">
+      <c r="A37" t="s" s="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" s="46" customFormat="true">
+      <c r="A38" t="s" s="46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" s="47" customFormat="true">
+      <c r="A39" t="s" s="47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" s="48" customFormat="true">
+      <c r="A40" t="s" s="48">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" s="49" customFormat="true">
+      <c r="A41" t="s" s="49">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" s="51" customFormat="true">
+      <c r="A42" t="s" s="51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s">
+    <row r="44">
+      <c r="A44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s">
+    <row r="45">
+      <c r="A45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s">
+    <row r="46">
+      <c r="A46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s">
+    <row r="47">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s">
+    <row r="50">
+      <c r="A50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" s="16" customFormat="true">
-      <c r="A37" t="s" s="16">
+    <row r="51" s="52" customFormat="true">
+      <c r="A51" t="s" s="52">
         <v>14</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s">
+    <row r="52" s="53" customFormat="true">
+      <c r="A52" t="s" s="53">
         <v>15</v>
       </c>
     </row>
-    <row r="39" s="17" customFormat="true">
-      <c r="A39" t="s" s="17">
+    <row r="53" s="55" customFormat="true">
+      <c r="A53" t="s" s="55">
         <v>16</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s">
+    <row r="54">
+      <c r="A54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>59</v>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="list" sqref="B3:F3" allowBlank="true" errorStyle="stop">
+  <dataValidations count="22">
+    <dataValidation type="list" sqref="B3:SG3" allowBlank="true" errorStyle="stop">
       <formula1>Place!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B13:F13" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B13:SG13" allowBlank="true" errorStyle="stop">
       <formula1>Activity!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B29:F29" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B21:SG21" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B22:SG22" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B23:SG23" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B24:SG24" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B25:SG25" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B26:SG26" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B36:SG36" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B37:SG37" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B38:SG38" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B39:SG39" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B40:SG40" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B41:SG41" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B43:SG43" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B30:F30" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B44:SG44" allowBlank="true" errorStyle="stop">
       <formula1>Architecture!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B31:F31" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B45:SG45" allowBlank="true" errorStyle="stop">
       <formula1>Person!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B32:F32" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B46:SG46" allowBlank="true" errorStyle="stop">
       <formula1>Group!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B33:F33" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B47:SG47" allowBlank="true" errorStyle="stop">
       <formula1>Institution!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B34:F34" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B48:SG48" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B41:F41" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B52:SG52" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B55:SG55" allowBlank="true" errorStyle="stop">
       <formula1>Object!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
@@ -909,143 +1581,143 @@
   <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.04296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="24.65625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="true">
-      <c r="A1" t="s" s="18">
+    <row r="1" s="56" customFormat="true">
+      <c r="A1" t="s" s="56">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="19" customFormat="true">
-      <c r="A2" t="s" s="19">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" s="20" customFormat="true">
-      <c r="A4" t="s" s="20">
+    <row r="2" s="57" customFormat="true">
+      <c r="A2" t="s" s="57">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" s="58" customFormat="true">
+      <c r="A3" t="s" s="58">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" s="60" customFormat="true">
+      <c r="A4" t="s" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" s="21" customFormat="true">
-      <c r="A6" t="s" s="21">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="6" s="61" customFormat="true">
+      <c r="A6" t="s" s="61">
         <v>65</v>
       </c>
     </row>
-    <row r="9" s="22" customFormat="true">
-      <c r="A9" t="s" s="22">
+    <row r="7" s="62" customFormat="true">
+      <c r="A7" t="s" s="62">
         <v>66</v>
+      </c>
+    </row>
+    <row r="8" s="63" customFormat="true">
+      <c r="A8" t="s" s="63">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" s="65" customFormat="true">
+      <c r="A9" t="s" s="65">
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" s="23" customFormat="true">
-      <c r="A15" t="s" s="23">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" s="24" customFormat="true">
-      <c r="A17" t="s" s="24">
+    <row r="15" s="66" customFormat="true">
+      <c r="A15" t="s" s="66">
         <v>74</v>
+      </c>
+    </row>
+    <row r="16" s="67" customFormat="true">
+      <c r="A16" t="s" s="67">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" s="69" customFormat="true">
+      <c r="A17" t="s" s="69">
+        <v>76</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" s="25" customFormat="true">
-      <c r="A19" t="s" s="25">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="19" s="70" customFormat="true">
+      <c r="A19" t="s" s="70">
         <v>78</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="20" s="71" customFormat="true">
+      <c r="A20" t="s" s="71">
         <v>79</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="21" s="72" customFormat="true">
+      <c r="A21" t="s" s="72">
         <v>80</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="22" s="73" customFormat="true">
+      <c r="A22" t="s" s="73">
         <v>81</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="23" s="74" customFormat="true">
+      <c r="A23" t="s" s="74">
         <v>82</v>
       </c>
     </row>
-    <row r="26" s="26" customFormat="true">
-      <c r="A26" t="s" s="26">
-        <v>75</v>
+    <row r="24" s="75" customFormat="true">
+      <c r="A24" t="s" s="75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" s="76" customFormat="true">
+      <c r="A25" t="s" s="76">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" s="78" customFormat="true">
+      <c r="A26" t="s" s="78">
+        <v>77</v>
       </c>
     </row>
     <row r="27">
@@ -1054,12 +1726,36 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" sqref="B13:F13" allowBlank="true" errorStyle="stop">
+  <dataValidations count="10">
+    <dataValidation type="list" sqref="B7:SG7" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B8:SG8" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B13:SG13" allowBlank="true" errorStyle="stop">
       <formula1>Institution!$B$1:$XFD$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="B14:F14" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="B14:SG14" allowBlank="true" errorStyle="stop">
       <formula1>Institution!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B20:SG20" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B21:SG21" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B22:SG22" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B23:SG23" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B24:SG24" allowBlank="true" errorStyle="stop">
+      <formula1>Activity!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B25:SG25" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1068,96 +1764,893 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="45.1171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true">
-      <c r="A1" t="s" s="27">
+    <row r="1" s="79" customFormat="true">
+      <c r="A1" t="s" s="79">
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" s="80" customFormat="true">
+      <c r="A5" t="s" s="80">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" s="81" customFormat="true">
+      <c r="A6" t="s" s="81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="82" customFormat="true">
+      <c r="A7" t="s" s="82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" s="83" customFormat="true">
+      <c r="A8" t="s" s="83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" s="85" customFormat="true">
+      <c r="A9" t="s" s="85">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" s="86" customFormat="true">
+      <c r="A13" t="s" s="86">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" s="87" customFormat="true">
+      <c r="A14" t="s" s="87">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" s="88" customFormat="true">
+      <c r="A15" t="s" s="88">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" s="90" customFormat="true">
+      <c r="A16" t="s" s="90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" s="91" customFormat="true">
+      <c r="A17" t="s" s="91">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" s="92" customFormat="true">
+      <c r="A18" t="s" s="92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" s="93" customFormat="true">
+      <c r="A19" t="s" s="93">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" s="95" customFormat="true">
+      <c r="A20" t="s" s="95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" s="96" customFormat="true">
+      <c r="A21" t="s" s="96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" s="97" customFormat="true">
+      <c r="A22" t="s" s="97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" s="99" customFormat="true">
+      <c r="A23" t="s" s="99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" s="100" customFormat="true">
+      <c r="A24" t="s" s="100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" s="101" customFormat="true">
+      <c r="A25" t="s" s="101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" s="103" customFormat="true">
+      <c r="A26" t="s" s="103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" s="104" customFormat="true">
+      <c r="A27" t="s" s="104">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" s="105" customFormat="true">
+      <c r="A28" t="s" s="105">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" s="106" customFormat="true">
+      <c r="A29" t="s" s="106">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" s="107" customFormat="true">
+      <c r="A30" t="s" s="107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" s="108" customFormat="true">
+      <c r="A31" t="s" s="108">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" s="110" customFormat="true">
+      <c r="A32" t="s" s="110">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" s="111" customFormat="true">
+      <c r="A37" t="s" s="111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" s="113" customFormat="true">
+      <c r="A38" t="s" s="113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" s="114" customFormat="true">
+      <c r="A39" t="s" s="114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" s="115" customFormat="true">
+      <c r="A40" t="s" s="115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" s="116" customFormat="true">
+      <c r="A41" t="s" s="116">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" s="117" customFormat="true">
+      <c r="A42" t="s" s="117">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" s="119" customFormat="true">
+      <c r="A43" t="s" s="119">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" s="120" customFormat="true">
+      <c r="A44" t="s" s="120">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" s="121" customFormat="true">
+      <c r="A45" t="s" s="121">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" s="122" customFormat="true">
+      <c r="A46" t="s" s="122">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" s="124" customFormat="true">
+      <c r="A47" t="s" s="124">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" s="125" customFormat="true">
+      <c r="A56" t="s" s="125">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" s="126" customFormat="true">
+      <c r="A57" t="s" s="126">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" s="128" customFormat="true">
+      <c r="A58" t="s" s="128">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation type="list" sqref="B10:SG10" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B11:SG11" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B14:SG14" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B15:SG15" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B21:SG21" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B33:SG33" allowBlank="true" errorStyle="stop">
+      <formula1>Institution!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B35:SG35" allowBlank="true" errorStyle="stop">
+      <formula1>Institution!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B36:SG36" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B44:SG44" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B45:SG45" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B46:SG46" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B47:SG47" allowBlank="true" errorStyle="stop">
+      <formula1>Group!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B49:SG49" allowBlank="true" errorStyle="stop">
+      <formula1>Activity!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B50:SG50" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B51:SG51" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B52:SG52" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B53:SG53" allowBlank="true" errorStyle="stop">
+      <formula1>Activity!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B57:SG57" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="28" customFormat="true">
-      <c r="A1" t="s" s="28">
+    <row r="1" s="129" customFormat="true">
+      <c r="A1" t="s" s="129">
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" sqref="B3:SG3" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B4:SG4" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B6:SG6" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B7:SG7" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="35.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true">
-      <c r="A1" t="s" s="29">
+    <row r="1" s="130" customFormat="true">
+      <c r="A1" t="s" s="130">
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" s="131" customFormat="true">
+      <c r="A7" t="s" s="131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" s="133" customFormat="true">
+      <c r="A8" t="s" s="133">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" s="134" customFormat="true">
+      <c r="A9" t="s" s="134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" s="135" customFormat="true">
+      <c r="A10" t="s" s="135">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" s="136" customFormat="true">
+      <c r="A11" t="s" s="136">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" s="138" customFormat="true">
+      <c r="A12" t="s" s="138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" s="139" customFormat="true">
+      <c r="A13" t="s" s="139">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" s="140" customFormat="true">
+      <c r="A14" t="s" s="140">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" s="142" customFormat="true">
+      <c r="A15" t="s" s="142">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" s="143" customFormat="true">
+      <c r="A16" t="s" s="143">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" s="145" customFormat="true">
+      <c r="A17" t="s" s="145">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" s="146" customFormat="true">
+      <c r="A18" t="s" s="146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" s="147" customFormat="true">
+      <c r="A19" t="s" s="147">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" s="148" customFormat="true">
+      <c r="A20" t="s" s="148">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" s="150" customFormat="true">
+      <c r="A21" t="s" s="150">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" s="152" customFormat="true">
+      <c r="A22" t="s" s="152">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" s="153" customFormat="true">
+      <c r="A26" t="s" s="153">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" s="154" customFormat="true">
+      <c r="A27" t="s" s="154">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" s="156" customFormat="true">
+      <c r="A28" t="s" s="156">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" s="157" customFormat="true">
+      <c r="A29" t="s" s="157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" s="158" customFormat="true">
+      <c r="A30" t="s" s="158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" s="159" customFormat="true">
+      <c r="A31" t="s" s="159">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" s="161" customFormat="true">
+      <c r="A32" t="s" s="161">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" s="163" customFormat="true">
+      <c r="A33" t="s" s="163">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" s="164" customFormat="true">
+      <c r="A34" t="s" s="164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="165" customFormat="true">
+      <c r="A35" t="s" s="165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" s="166" customFormat="true">
+      <c r="A36" t="s" s="166">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" s="168" customFormat="true">
+      <c r="A37" t="s" s="168">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" s="169" customFormat="true">
+      <c r="A51" t="s" s="169">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" s="170" customFormat="true">
+      <c r="A52" t="s" s="170">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" s="172" customFormat="true">
+      <c r="A53" t="s" s="172">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="15">
+    <dataValidation type="list" sqref="B13:SG13" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B14:SG14" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B15:SG15" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B22:SG22" allowBlank="true" errorStyle="stop">
+      <formula1>Place!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B27:SG27" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B38:SG38" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B39:SG39" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B40:SG40" allowBlank="true" errorStyle="stop">
+      <formula1>Activity!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B41:SG41" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B42:SG42" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B43:SG43" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B47:SG47" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B48:SG48" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B52:SG52" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B55:SG55" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="23.58984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="true">
-      <c r="A1" t="s" s="30">
+    <row r="1" s="173" customFormat="true">
+      <c r="A1" t="s" s="173">
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" s="174" customFormat="true">
+      <c r="A10" t="s" s="174">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" s="175" customFormat="true">
+      <c r="A11" t="s" s="175">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" s="177" customFormat="true">
+      <c r="A12" t="s" s="177">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="list" sqref="B4:SG4" allowBlank="true" errorStyle="stop">
+      <formula1>Architecture!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B5:SG5" allowBlank="true" errorStyle="stop">
+      <formula1>Activity!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B6:SG6" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B7:SG7" allowBlank="true" errorStyle="stop">
+      <formula1>Person!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B11:SG11" allowBlank="true" errorStyle="stop">
+      <formula1>Reference!$B$1:$XFD$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B14:SG14" allowBlank="true" errorStyle="stop">
+      <formula1>Object!$B$1:$XFD$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Intermediate push; ExcelParser prototype ready but not tested properly
</commit_message>
<xml_diff>
--- a/templates/visitExcel.xlsx
+++ b/templates/visitExcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -30,268 +30,313 @@
     <t>Beschreibung</t>
   </si>
   <si>
+    <t>Datierung - Untergruppe</t>
+  </si>
+  <si>
+    <t>Taggenaue Datierung</t>
+  </si>
+  <si>
+    <t>Freie Datierung</t>
+  </si>
+  <si>
+    <t>Beginn des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Ende des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t>Beteiligte Personen</t>
+  </si>
+  <si>
+    <t>Beteiligte Bauwerke</t>
+  </si>
+  <si>
+    <t>Beteiligtes Objekt</t>
+  </si>
+  <si>
+    <t>Schlagwort</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Literaturangaben - Untergruppe</t>
+  </si>
+  <si>
+    <t>Kurztitel</t>
+  </si>
+  <si>
+    <t>Seiten</t>
+  </si>
+  <si>
+    <t>Hilfreiche Links</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Werkstatt</t>
+  </si>
+  <si>
+    <t>Besitz, Bauwerk</t>
+  </si>
+  <si>
+    <t>In Auftrag gegebene Bauwerke</t>
+  </si>
+  <si>
+    <t>Ausgeführte Bauwerke</t>
+  </si>
+  <si>
+    <t>Beteiligt an, Bauwerk</t>
+  </si>
+  <si>
+    <t>In Auftrag gegebene Baumaßnahmen</t>
+  </si>
+  <si>
+    <t>Ausgeführte Baumaßnahmen</t>
+  </si>
+  <si>
+    <t>Beteiligt an, Baumaßnahmen</t>
+  </si>
+  <si>
+    <t>Im Besitz befindliche Objekte</t>
+  </si>
+  <si>
+    <t>Ehemals im Besitz befindliche Objekte</t>
+  </si>
+  <si>
+    <t>Standort</t>
+  </si>
+  <si>
+    <t>Geographische Zuordnung</t>
+  </si>
+  <si>
+    <t>Kirchliche Gliederung</t>
+  </si>
+  <si>
+    <t>Ordenszugehörigkeit</t>
+  </si>
+  <si>
+    <t>Sakralbau</t>
+  </si>
+  <si>
+    <t>Profanbau</t>
+  </si>
+  <si>
+    <t>Innere Baubeschreibung</t>
+  </si>
+  <si>
+    <t>Äußere Baubeschreibung</t>
+  </si>
+  <si>
+    <t>Funktion</t>
+  </si>
+  <si>
+    <t>Geschichte</t>
+  </si>
+  <si>
+    <t>Ereignis</t>
+  </si>
+  <si>
+    <t>Baugeschichte</t>
+  </si>
+  <si>
+    <t>Bau - Untergruppe</t>
+  </si>
+  <si>
+    <t>Datierung - Bau</t>
+  </si>
+  <si>
+    <t>Datierung - Bau - Unteruntergruppe</t>
+  </si>
+  <si>
+    <t>Entstehung: Beginn des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Entstehung: Ende des Datierungszeitraums</t>
+  </si>
+  <si>
+    <t>Entstehung: Freie Datierung</t>
+  </si>
+  <si>
+    <t>Entstehung: Jahrhundert</t>
+  </si>
+  <si>
+    <t>Auftraggeber Person - Bau</t>
+  </si>
+  <si>
+    <t>Ausführende Personen - Bau</t>
+  </si>
+  <si>
+    <t>Beteiligte Personen - Bau</t>
+  </si>
+  <si>
+    <t>Auftraggeber Gruppe - Bau</t>
+  </si>
+  <si>
+    <t>Ausführende Gruppe - Bau</t>
+  </si>
+  <si>
+    <t>Beteiligte Gruppe - Bau</t>
+  </si>
+  <si>
+    <t>Bauphasen - Untergruppe</t>
+  </si>
+  <si>
+    <t>Datierung - Bauphase</t>
+  </si>
+  <si>
+    <t>Datierung - Bauphase - Unteruntergruppe</t>
+  </si>
+  <si>
+    <t>Beginn der Bauphase</t>
+  </si>
+  <si>
+    <t>Ende der Bauphase</t>
+  </si>
+  <si>
+    <t>Jahrhundert</t>
+  </si>
+  <si>
+    <t>Funktion - Bauphase</t>
+  </si>
+  <si>
+    <t>Auftraggeber Person - Bauphase</t>
+  </si>
+  <si>
+    <t>Ausführende Personen - Bauphase</t>
+  </si>
+  <si>
+    <t>Beteiligte Personen - Bauphase</t>
+  </si>
+  <si>
+    <t>Auftraggeber Gruppe - Bauphase</t>
+  </si>
+  <si>
+    <t>Ausführende Gruppe - Bauphase</t>
+  </si>
+  <si>
+    <t>Beteiligte Gruppe - Bauphase</t>
+  </si>
+  <si>
+    <t>Kommentar - Bauphase</t>
+  </si>
+  <si>
+    <t>Enthaltene Bauteile</t>
+  </si>
+  <si>
+    <t>Bauteil von</t>
+  </si>
+  <si>
+    <t>Eigentümer/Verwalter Person</t>
+  </si>
+  <si>
+    <t>Eigentümer/Verwalter Gruppe</t>
+  </si>
+  <si>
+    <t>Eigentümer/Verwalter Institution</t>
+  </si>
+  <si>
+    <t>Enthaltene Objekte</t>
+  </si>
+  <si>
+    <t>Darstellung</t>
+  </si>
+  <si>
+    <t>Titelangaben - Untergruppe</t>
+  </si>
+  <si>
+    <t>Übergeordneter Titel</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Autor, Jahr, Ort - Kurztitel - Untergruppe</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Erscheinungsort</t>
+  </si>
+  <si>
+    <t>Erscheinungsjahr</t>
+  </si>
+  <si>
+    <t>Herausgeber</t>
+  </si>
+  <si>
+    <t>Bandzahl</t>
+  </si>
+  <si>
+    <t>Reihe</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Ort der Ausstellung</t>
+  </si>
+  <si>
+    <t>Jahr der Ausstellung - Untergruppe</t>
+  </si>
+  <si>
+    <t>Beginn der Ausstellung</t>
+  </si>
+  <si>
+    <t>Ende der Ausstellung</t>
+  </si>
+  <si>
+    <t>Seite/n</t>
+  </si>
+  <si>
+    <t>Verweis auf - Untergruppe</t>
+  </si>
+  <si>
+    <t>Verweis auf Objekt</t>
+  </si>
+  <si>
+    <t>Verweis auf Bauwerk</t>
+  </si>
+  <si>
+    <t>Verweis auf Gruppe</t>
+  </si>
+  <si>
+    <t>Verweis auf Person</t>
+  </si>
+  <si>
+    <t>Verweis auf Ereignis</t>
+  </si>
+  <si>
+    <t>Verweis auf Ort</t>
+  </si>
+  <si>
+    <t>Objektbezeichnung</t>
+  </si>
+  <si>
+    <t>Allgemeine Objektdatierung - Untergruppe</t>
+  </si>
+  <si>
+    <t>Objekt besteht aus Teilobjekten</t>
+  </si>
+  <si>
+    <t>Teilobjekt von</t>
+  </si>
+  <si>
+    <t>Herstellung - Untergruppe</t>
+  </si>
+  <si>
+    <t>Künstler</t>
+  </si>
+  <si>
     <t>Datierung</t>
   </si>
   <si>
-    <t>Taggenaue Datierung</t>
-  </si>
-  <si>
-    <t>Freie Datierung</t>
-  </si>
-  <si>
-    <t>Beginn des Datierungszeitraums</t>
-  </si>
-  <si>
-    <t>Ende des Datierungszeitraums</t>
-  </si>
-  <si>
-    <t>Ort</t>
-  </si>
-  <si>
-    <t>Beteiligte Personen</t>
-  </si>
-  <si>
-    <t>Beteiligte Bauwerke</t>
-  </si>
-  <si>
-    <t>Beteiligtes Objekt</t>
-  </si>
-  <si>
-    <t>Schlagwort</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Literaturangaben</t>
-  </si>
-  <si>
-    <t>Kurztitel</t>
-  </si>
-  <si>
-    <t>Seiten</t>
-  </si>
-  <si>
-    <t>Hilfreiche Links</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Werkstatt</t>
-  </si>
-  <si>
-    <t>Besitz, Bauwerk</t>
-  </si>
-  <si>
-    <t>In Auftrag gegebene Bauwerke</t>
-  </si>
-  <si>
-    <t>Ausgeführte Bauwerke</t>
-  </si>
-  <si>
-    <t>Beteiligt an, Bauwerk</t>
-  </si>
-  <si>
-    <t>In Auftrag gegebene Baumaßnahmen</t>
-  </si>
-  <si>
-    <t>Ausgeführte Baumaßnahmen</t>
-  </si>
-  <si>
-    <t>Beteiligt an, Baumaßnahmen</t>
-  </si>
-  <si>
-    <t>Im Besitz befindliche Objekte</t>
-  </si>
-  <si>
-    <t>Ehemals im Besitz befindliche Objekte</t>
-  </si>
-  <si>
-    <t>Standort</t>
-  </si>
-  <si>
-    <t>Geographische Zuordnung</t>
-  </si>
-  <si>
-    <t>Kirchliche Gliederung</t>
-  </si>
-  <si>
-    <t>Ordenszugehörigkeit</t>
-  </si>
-  <si>
-    <t>Sakralbau</t>
-  </si>
-  <si>
-    <t>Profanbau</t>
-  </si>
-  <si>
-    <t>Innere Baubeschreibung</t>
-  </si>
-  <si>
-    <t>Äußere Baubeschreibung</t>
-  </si>
-  <si>
-    <t>Funktion</t>
-  </si>
-  <si>
-    <t>Geschichte</t>
-  </si>
-  <si>
-    <t>Ereignis</t>
-  </si>
-  <si>
-    <t>Baugeschichte</t>
-  </si>
-  <si>
-    <t>Bau</t>
-  </si>
-  <si>
-    <t>Entstehung:Beginn des Datierungszeitraums</t>
-  </si>
-  <si>
-    <t>Entstehung: Ende des Datierungszeitraums</t>
-  </si>
-  <si>
-    <t>Entstehung: Freie Datierung</t>
-  </si>
-  <si>
-    <t>Entstehung: Jahrhundert</t>
-  </si>
-  <si>
-    <t>Auftraggeber Person</t>
-  </si>
-  <si>
-    <t>Ausführende Personen</t>
-  </si>
-  <si>
-    <t>Auftraggeber Gruppe</t>
-  </si>
-  <si>
-    <t>Ausführende Gruppe</t>
-  </si>
-  <si>
-    <t>Beteiligte Gruppe</t>
-  </si>
-  <si>
-    <t>Bauphasen</t>
-  </si>
-  <si>
-    <t>Beginn der Bauphase</t>
-  </si>
-  <si>
-    <t>Ende der Bauphase</t>
-  </si>
-  <si>
-    <t>Jahrhundert</t>
-  </si>
-  <si>
-    <t>Enthaltene Bauteile</t>
-  </si>
-  <si>
-    <t>Bauteil von</t>
-  </si>
-  <si>
-    <t>Eigentümer/Verwalter Person</t>
-  </si>
-  <si>
-    <t>Eigentümer/Verwalter Gruppe</t>
-  </si>
-  <si>
-    <t>Eigentümer/Verwalter Institution</t>
-  </si>
-  <si>
-    <t>Enthaltene Objekte</t>
-  </si>
-  <si>
-    <t>Darstellung</t>
-  </si>
-  <si>
-    <t>Titelangaben</t>
-  </si>
-  <si>
-    <t>Übergeordneter Titel</t>
-  </si>
-  <si>
-    <t>Typ</t>
-  </si>
-  <si>
-    <t>Autor, Jahr, Ort - Kurztitel</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>Erscheinungsort</t>
-  </si>
-  <si>
-    <t>Erscheinungsjahr</t>
-  </si>
-  <si>
-    <t>Herausgeber</t>
-  </si>
-  <si>
-    <t>Bandzahl</t>
-  </si>
-  <si>
-    <t>Reihe</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Ort der Ausstellung</t>
-  </si>
-  <si>
-    <t>Jahr der Ausstellung</t>
-  </si>
-  <si>
-    <t>Beginn der Ausstellung</t>
-  </si>
-  <si>
-    <t>Ende der Ausstellung</t>
-  </si>
-  <si>
-    <t>Seite/n</t>
-  </si>
-  <si>
-    <t>Verweis auf</t>
-  </si>
-  <si>
-    <t>Verweis auf Objekt</t>
-  </si>
-  <si>
-    <t>Verweis auf Bauwerk</t>
-  </si>
-  <si>
-    <t>Verweis auf Gruppe</t>
-  </si>
-  <si>
-    <t>Verweis auf Person</t>
-  </si>
-  <si>
-    <t>Verweis auf Ereignis</t>
-  </si>
-  <si>
-    <t>Verweis auf Ort</t>
-  </si>
-  <si>
-    <t>Objektbezeichnung</t>
-  </si>
-  <si>
-    <t>Allgemeine Objektdatierung</t>
-  </si>
-  <si>
-    <t>Objekt besteht aus Teilobjekten</t>
-  </si>
-  <si>
-    <t>Teilobjekt von</t>
-  </si>
-  <si>
-    <t>Herstellung</t>
-  </si>
-  <si>
-    <t>Künstler</t>
+    <t>Datierung - Unteruntergruppe</t>
   </si>
   <si>
     <t>Entstehungszeit: Freie Datierung</t>
@@ -315,7 +360,7 @@
     <t>Technik</t>
   </si>
   <si>
-    <t>Masse</t>
+    <t>Masse - Untergruppe</t>
   </si>
   <si>
     <t>Abmessung</t>
@@ -324,7 +369,7 @@
     <t>Wert</t>
   </si>
   <si>
-    <t>Inschrift</t>
+    <t>Inschrift - Untergruppe</t>
   </si>
   <si>
     <t>Art</t>
@@ -351,12 +396,15 @@
     <t>Standort - Bauwerk</t>
   </si>
   <si>
-    <t>Provenienz</t>
+    <t>Provenienz - Untergruppe</t>
   </si>
   <si>
     <t>Datierung des Besitzerwechsels</t>
   </si>
   <si>
+    <t>Datierung des Besitzerwechsels - Unteruntergruppe</t>
+  </si>
+  <si>
     <t>Eigentümer - Person</t>
   </si>
   <si>
@@ -411,12 +459,15 @@
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>Geburt</t>
+    <t>Geburt - Untergruppe</t>
   </si>
   <si>
     <t>Geburtsdatum</t>
   </si>
   <si>
+    <t>Geburtsdatum - Unteruntergruppe</t>
+  </si>
+  <si>
     <t>Geburtsort</t>
   </si>
   <si>
@@ -426,19 +477,22 @@
     <t>Vater</t>
   </si>
   <si>
-    <t>Tod</t>
+    <t>Tod - Untergruppe</t>
   </si>
   <si>
     <t>Sterbedatum</t>
   </si>
   <si>
+    <t>Sterbedatum - Unteruntergruppe</t>
+  </si>
+  <si>
     <t>Sterbeort</t>
   </si>
   <si>
     <t>Amt/Beruf</t>
   </si>
   <si>
-    <t>Ehe</t>
+    <t>Ehe - Untergruppe</t>
   </si>
   <si>
     <t>Ehepartner</t>
@@ -447,7 +501,13 @@
     <t>Beginn der Ehe</t>
   </si>
   <si>
+    <t>Beginn der Ehe - Unteruntergruppe</t>
+  </si>
+  <si>
     <t>Ende der Ehe</t>
+  </si>
+  <si>
+    <t>Ende der Ehe - Unteruntergruppe</t>
   </si>
   <si>
     <t>Kinder</t>
@@ -974,7 +1034,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.8046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.26171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true">
@@ -1225,7 +1285,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="41.05078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true">
@@ -1305,62 +1365,62 @@
     </row>
     <row r="16" s="20" customFormat="true">
       <c r="A16" t="s" s="20">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" s="21" customFormat="true">
       <c r="A17" t="s" s="21">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" s="22" customFormat="true">
       <c r="A18" t="s" s="22">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" s="23" customFormat="true">
       <c r="A19" t="s" s="23">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" s="25" customFormat="true">
       <c r="A20" t="s" s="25">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" s="26" customFormat="true">
       <c r="A21" t="s" s="26">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" s="27" customFormat="true">
       <c r="A22" t="s" s="27">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" s="28" customFormat="true">
       <c r="A23" t="s" s="28">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" s="29" customFormat="true">
       <c r="A24" t="s" s="29">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" s="30" customFormat="true">
       <c r="A25" t="s" s="30">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" s="32" customFormat="true">
       <c r="A26" t="s" s="32">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" s="33" customFormat="true">
       <c r="A27" t="s" s="33">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" s="34" customFormat="true">
@@ -1370,17 +1430,17 @@
     </row>
     <row r="29" s="36" customFormat="true">
       <c r="A29" t="s" s="36">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" s="37" customFormat="true">
       <c r="A30" t="s" s="37">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" s="38" customFormat="true">
       <c r="A31" t="s" s="38">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" s="39" customFormat="true">
@@ -1390,7 +1450,7 @@
     </row>
     <row r="33" s="41" customFormat="true">
       <c r="A33" t="s" s="41">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" s="42" customFormat="true">
@@ -1400,72 +1460,72 @@
     </row>
     <row r="35" s="43" customFormat="true">
       <c r="A35" t="s" s="43">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" s="44" customFormat="true">
       <c r="A36" t="s" s="44">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" s="45" customFormat="true">
       <c r="A37" t="s" s="45">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" s="46" customFormat="true">
       <c r="A38" t="s" s="46">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" s="47" customFormat="true">
       <c r="A39" t="s" s="47">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" s="48" customFormat="true">
       <c r="A40" t="s" s="48">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" s="49" customFormat="true">
       <c r="A41" t="s" s="49">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" s="51" customFormat="true">
       <c r="A42" t="s" s="51">
-        <v>13</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49">
@@ -1500,7 +1560,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1647,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.65625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.06640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="56" customFormat="true">
@@ -1597,12 +1657,12 @@
     </row>
     <row r="2" s="57" customFormat="true">
       <c r="A2" t="s" s="57">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" s="58" customFormat="true">
       <c r="A3" t="s" s="58">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" s="60" customFormat="true">
@@ -1612,112 +1672,112 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" s="61" customFormat="true">
       <c r="A6" t="s" s="61">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" s="62" customFormat="true">
       <c r="A7" t="s" s="62">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" s="63" customFormat="true">
       <c r="A8" t="s" s="63">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" s="65" customFormat="true">
       <c r="A9" t="s" s="65">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" s="66" customFormat="true">
       <c r="A15" t="s" s="66">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" s="67" customFormat="true">
       <c r="A16" t="s" s="67">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" s="69" customFormat="true">
       <c r="A17" t="s" s="69">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" s="70" customFormat="true">
       <c r="A19" t="s" s="70">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" s="71" customFormat="true">
       <c r="A20" t="s" s="71">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" s="72" customFormat="true">
       <c r="A21" t="s" s="72">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" s="73" customFormat="true">
       <c r="A22" t="s" s="73">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" s="74" customFormat="true">
       <c r="A23" t="s" s="74">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" s="75" customFormat="true">
       <c r="A24" t="s" s="75">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" s="76" customFormat="true">
       <c r="A25" t="s" s="76">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" s="78" customFormat="true">
       <c r="A26" t="s" s="78">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
@@ -1773,7 +1833,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.1171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="48.24609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="79" customFormat="true">
@@ -1788,7 +1848,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
@@ -1798,7 +1858,7 @@
     </row>
     <row r="5" s="80" customFormat="true">
       <c r="A5" t="s" s="80">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" s="81" customFormat="true">
@@ -1818,17 +1878,17 @@
     </row>
     <row r="9" s="85" customFormat="true">
       <c r="A9" t="s" s="85">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
@@ -1838,12 +1898,12 @@
     </row>
     <row r="13" s="86" customFormat="true">
       <c r="A13" t="s" s="86">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" s="87" customFormat="true">
       <c r="A14" t="s" s="87">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" s="88" customFormat="true">
@@ -1853,117 +1913,117 @@
     </row>
     <row r="16" s="90" customFormat="true">
       <c r="A16" t="s" s="90">
-        <v>3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" s="91" customFormat="true">
       <c r="A17" t="s" s="91">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" s="92" customFormat="true">
       <c r="A18" t="s" s="92">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" s="93" customFormat="true">
       <c r="A19" t="s" s="93">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" s="95" customFormat="true">
       <c r="A20" t="s" s="95">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" s="96" customFormat="true">
       <c r="A21" t="s" s="96">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" s="97" customFormat="true">
       <c r="A22" t="s" s="97">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" s="99" customFormat="true">
       <c r="A23" t="s" s="99">
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" s="100" customFormat="true">
       <c r="A24" t="s" s="100">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" s="101" customFormat="true">
       <c r="A25" t="s" s="101">
-        <v>99</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" s="103" customFormat="true">
       <c r="A26" t="s" s="103">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" s="104" customFormat="true">
       <c r="A27" t="s" s="104">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" s="105" customFormat="true">
       <c r="A28" t="s" s="105">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" s="106" customFormat="true">
       <c r="A29" t="s" s="106">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" s="107" customFormat="true">
       <c r="A30" t="s" s="107">
-        <v>3</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" s="108" customFormat="true">
       <c r="A31" t="s" s="108">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" s="110" customFormat="true">
       <c r="A32" t="s" s="110">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" s="111" customFormat="true">
       <c r="A37" t="s" s="111">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" s="113" customFormat="true">
       <c r="A38" t="s" s="113">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" s="114" customFormat="true">
@@ -1988,57 +2048,57 @@
     </row>
     <row r="43" s="119" customFormat="true">
       <c r="A43" t="s" s="119">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" s="120" customFormat="true">
       <c r="A44" t="s" s="120">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" s="121" customFormat="true">
       <c r="A45" t="s" s="121">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" s="122" customFormat="true">
       <c r="A46" t="s" s="122">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" s="124" customFormat="true">
       <c r="A47" t="s" s="124">
-        <v>115</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54">
@@ -2158,7 +2218,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4">
@@ -2168,17 +2228,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8">
@@ -2226,37 +2286,37 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" s="131" customFormat="true">
       <c r="A7" t="s" s="131">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" s="133" customFormat="true">
       <c r="A8" t="s" s="133">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" s="134" customFormat="true">
@@ -2281,27 +2341,27 @@
     </row>
     <row r="13" s="139" customFormat="true">
       <c r="A13" t="s" s="139">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" s="140" customFormat="true">
       <c r="A14" t="s" s="140">
-        <v>133</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" s="142" customFormat="true">
       <c r="A15" t="s" s="142">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" s="143" customFormat="true">
       <c r="A16" t="s" s="143">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" s="145" customFormat="true">
       <c r="A17" t="s" s="145">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" s="146" customFormat="true">
@@ -2326,12 +2386,12 @@
     </row>
     <row r="22" s="152" customFormat="true">
       <c r="A22" t="s" s="152">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24">
@@ -2346,17 +2406,17 @@
     </row>
     <row r="26" s="153" customFormat="true">
       <c r="A26" t="s" s="153">
-        <v>139</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" s="154" customFormat="true">
       <c r="A27" t="s" s="154">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" s="156" customFormat="true">
       <c r="A28" t="s" s="156">
-        <v>141</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" s="157" customFormat="true">
@@ -2381,7 +2441,7 @@
     </row>
     <row r="33" s="163" customFormat="true">
       <c r="A33" t="s" s="163">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" s="164" customFormat="true">
@@ -2406,17 +2466,17 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41">
@@ -2431,7 +2491,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44">
@@ -2446,7 +2506,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47">
@@ -2491,7 +2551,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2617,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="23.58984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.26171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="173" customFormat="true">
@@ -2567,7 +2627,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
@@ -2577,7 +2637,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5">
@@ -2587,12 +2647,12 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8">
@@ -2627,7 +2687,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used Miriam's Input for IdMaps; Changed small thing for ExcelProducer
</commit_message>
<xml_diff>
--- a/templates/visitExcel.xlsx
+++ b/templates/visitExcel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -177,7 +177,7 @@
     <t>Auftraggeber Gruppe - Bau</t>
   </si>
   <si>
-    <t>Ausführende Gruppe - Bau</t>
+    <t>AusfÜhrende Gruppe - Bau</t>
   </si>
   <si>
     <t>Beteiligte Gruppe - Bau</t>
@@ -291,28 +291,31 @@
     <t>Ende der Ausstellung</t>
   </si>
   <si>
+    <t>Seitenzahl</t>
+  </si>
+  <si>
+    <t>Verweis auf - Untergruppe</t>
+  </si>
+  <si>
+    <t>Verweis auf Objekt</t>
+  </si>
+  <si>
+    <t>Verweis auf Bauwerk</t>
+  </si>
+  <si>
+    <t>Verweis auf Gruppe</t>
+  </si>
+  <si>
+    <t>Verweis auf Person</t>
+  </si>
+  <si>
+    <t>Verweis auf Ereignis</t>
+  </si>
+  <si>
+    <t>Verweis auf Ort</t>
+  </si>
+  <si>
     <t>Seite/n</t>
-  </si>
-  <si>
-    <t>Verweis auf - Untergruppe</t>
-  </si>
-  <si>
-    <t>Verweis auf Objekt</t>
-  </si>
-  <si>
-    <t>Verweis auf Bauwerk</t>
-  </si>
-  <si>
-    <t>Verweis auf Gruppe</t>
-  </si>
-  <si>
-    <t>Verweis auf Person</t>
-  </si>
-  <si>
-    <t>Verweis auf Ereignis</t>
-  </si>
-  <si>
-    <t>Verweis auf Ort</t>
   </si>
   <si>
     <t>Objektbezeichnung</t>
@@ -1777,7 +1780,7 @@
     </row>
     <row r="26" s="78" customFormat="true">
       <c r="A26" t="s" s="78">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27">
@@ -1848,7 +1851,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
@@ -1858,7 +1861,7 @@
     </row>
     <row r="5" s="80" customFormat="true">
       <c r="A5" t="s" s="80">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" s="81" customFormat="true">
@@ -1883,12 +1886,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
@@ -1898,12 +1901,12 @@
     </row>
     <row r="13" s="86" customFormat="true">
       <c r="A13" t="s" s="86">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" s="87" customFormat="true">
       <c r="A14" t="s" s="87">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" s="88" customFormat="true">
@@ -1913,117 +1916,117 @@
     </row>
     <row r="16" s="90" customFormat="true">
       <c r="A16" t="s" s="90">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" s="91" customFormat="true">
       <c r="A17" t="s" s="91">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" s="92" customFormat="true">
       <c r="A18" t="s" s="92">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" s="93" customFormat="true">
       <c r="A19" t="s" s="93">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" s="95" customFormat="true">
       <c r="A20" t="s" s="95">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" s="96" customFormat="true">
       <c r="A21" t="s" s="96">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" s="97" customFormat="true">
       <c r="A22" t="s" s="97">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" s="99" customFormat="true">
       <c r="A23" t="s" s="99">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" s="100" customFormat="true">
       <c r="A24" t="s" s="100">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" s="101" customFormat="true">
       <c r="A25" t="s" s="101">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" s="103" customFormat="true">
       <c r="A26" t="s" s="103">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" s="104" customFormat="true">
       <c r="A27" t="s" s="104">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" s="105" customFormat="true">
       <c r="A28" t="s" s="105">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" s="106" customFormat="true">
       <c r="A29" t="s" s="106">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" s="107" customFormat="true">
       <c r="A30" t="s" s="107">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" s="108" customFormat="true">
       <c r="A31" t="s" s="108">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" s="110" customFormat="true">
       <c r="A32" t="s" s="110">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" s="111" customFormat="true">
       <c r="A37" t="s" s="111">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" s="113" customFormat="true">
       <c r="A38" t="s" s="113">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" s="114" customFormat="true">
@@ -2053,22 +2056,22 @@
     </row>
     <row r="44" s="120" customFormat="true">
       <c r="A44" t="s" s="120">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" s="121" customFormat="true">
       <c r="A45" t="s" s="121">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" s="122" customFormat="true">
       <c r="A46" t="s" s="122">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" s="124" customFormat="true">
       <c r="A47" t="s" s="124">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48">
@@ -2078,27 +2081,27 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54">
@@ -2218,7 +2221,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4">
@@ -2228,17 +2231,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8">
@@ -2286,37 +2289,37 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" s="131" customFormat="true">
       <c r="A7" t="s" s="131">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" s="133" customFormat="true">
       <c r="A8" t="s" s="133">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" s="134" customFormat="true">
@@ -2341,27 +2344,27 @@
     </row>
     <row r="13" s="139" customFormat="true">
       <c r="A13" t="s" s="139">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" s="140" customFormat="true">
       <c r="A14" t="s" s="140">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" s="142" customFormat="true">
       <c r="A15" t="s" s="142">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" s="143" customFormat="true">
       <c r="A16" t="s" s="143">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" s="145" customFormat="true">
       <c r="A17" t="s" s="145">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" s="146" customFormat="true">
@@ -2386,12 +2389,12 @@
     </row>
     <row r="22" s="152" customFormat="true">
       <c r="A22" t="s" s="152">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24">
@@ -2406,17 +2409,17 @@
     </row>
     <row r="26" s="153" customFormat="true">
       <c r="A26" t="s" s="153">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" s="154" customFormat="true">
       <c r="A27" t="s" s="154">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" s="156" customFormat="true">
       <c r="A28" t="s" s="156">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" s="157" customFormat="true">
@@ -2441,7 +2444,7 @@
     </row>
     <row r="33" s="163" customFormat="true">
       <c r="A33" t="s" s="163">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" s="164" customFormat="true">
@@ -2466,17 +2469,17 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41">
@@ -2491,7 +2494,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44">
@@ -2506,7 +2509,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47">
@@ -2551,7 +2554,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2627,7 +2630,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
@@ -2637,7 +2640,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5">
@@ -2647,12 +2650,12 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8">
@@ -2687,7 +2690,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel file with locked cells
Password to unlock cells: visitExcel
</commit_message>
<xml_diff>
--- a/templates/visitExcel.xlsx
+++ b/templates/visitExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\metadata_api\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\metadata_rest_api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF44000C-669C-4D88-A794-3D4B30694A26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C045C17-2644-4576-B2C8-546B29E13060}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -894,152 +894,170 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1354,111 +1372,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Zdi+n3kLpgyXxWVUFtGFeTBrkyM8yajgqhbN4HnMiUxcvxEES9fEKiCDqmcxmwHS1/6z86hlxP59Jg2nNvqagg==" saltValue="7oM24y7se+A4hMl2SMAQPA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1501,101 +1554,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="/brE24o2Uska4ZDdTQG+OPjD0Yc2NCAvKsFlM6PiwTXMDuirJnbjvPS/adtMVo2oG7Qut46UVBCiSd3Q15ShwQ==" saltValue="ruiqJfz+lqsZhBCWx3XA4A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1632,290 +1726,292 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
+    <row r="31" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
+    <row r="32" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+    <row r="33" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35" t="s">
+    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37" t="s">
+    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="38" t="s">
+    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
+    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40" t="s">
+    <row r="40" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="41" t="s">
+    <row r="41" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="42" t="s">
+    <row r="42" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:1" s="43" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="43" t="s">
+    <row r="51" spans="1:1" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="44" t="s">
+    <row r="52" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="45" t="s">
+    <row r="53" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="doEANa0GKH1EaHXtmSUV9pcmfYkmqJ5Fs60EfbxQVWzw/dKqCkcbMZuVG0LFGAH2RVFsL7uk2snWhU2M4tvpbA==" saltValue="OR99wdhckZl1/pVUOS3v8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B43:SG44" xr:uid="{00000000-0002-0000-0200-00000E000000}">
       <formula1>$B$1:$XFD$1</formula1>
@@ -1975,156 +2071,164 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:1" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:1" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52" t="s">
+    <row r="8" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53" t="s">
+    <row r="9" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="s">
+    <row r="15" spans="1:1" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56" t="s">
+    <row r="17" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+    <row r="19" spans="1:1" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+    <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="59" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="59" t="s">
+    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="60" t="s">
+    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="61" t="s">
+    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62" t="s">
+    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="63" t="s">
+    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64" t="s">
+    <row r="26" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="xZn3/tru2QwXlEXtxBtBmN7wZhAgcqOmBuZ7gPCL/I/noJ91NzTGDEOO+Fcp9NuH9/aKJFdD6MkJZRqa8SzxaA==" saltValue="dOLOimoQGJ3c/VoRcUUsGA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2181,314 +2285,316 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T17" sqref="T17"/>
+      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="65" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="144" t="s">
+    <row r="1" spans="1:1" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="142" t="s">
+    <row r="5" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="67" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="140" t="s">
+    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="140" t="s">
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="140" t="s">
+    <row r="8" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="70" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="141" t="s">
+    <row r="9" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="142" t="s">
+    <row r="13" spans="1:1" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="140" t="s">
+    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="73" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="140" t="s">
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143" t="s">
+    <row r="16" spans="1:1" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="56" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="75" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="133" t="s">
+    <row r="17" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="76" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="133" t="s">
+    <row r="18" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="77" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="133" t="s">
+    <row r="19" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="134" t="s">
+    <row r="20" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="140" t="s">
+    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="80" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="140" t="s">
+    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="141" t="s">
+    <row r="23" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="142" t="s">
+    <row r="24" spans="1:1" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="55" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="83" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="140" t="s">
+    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="84" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="141" t="s">
+    <row r="26" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="142" t="s">
+    <row r="27" spans="1:1" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="55" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="86" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="140" t="s">
+    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="87" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="140" t="s">
+    <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="88" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="140" t="s">
+    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="89" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="140" t="s">
+    <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="90" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="141" t="s">
+    <row r="32" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="91" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="142" t="s">
+    <row r="37" spans="1:1" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="55" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="92" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="143" t="s">
+    <row r="38" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="56" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="93" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="133" t="s">
+    <row r="39" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="133" t="s">
+    <row r="40" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="95" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="133" t="s">
+    <row r="41" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="96" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="133" t="s">
+    <row r="42" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:1" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="134" t="s">
+    <row r="43" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="31" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:1" s="98" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="140" t="s">
+    <row r="44" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="99" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="140" t="s">
+    <row r="45" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="140" t="s">
+    <row r="46" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:1" s="101" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="141" t="s">
+    <row r="47" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:1" s="102" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="142" t="s">
+    <row r="56" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:1" s="103" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="140" t="s">
+    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:1" s="104" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="141" t="s">
+    <row r="58" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vuaofta2QNWkHPgQ3D/tXDSMnsfd3Og2EgHwIYouvOhbX76fL1vF4TGdKgXmQzE4ZZV9tLQ+g/6KDY0uMHaUNw==" saltValue="bmpFNOPUpE9ZlH96Mb2F8g==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B10:SG11" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$B$1:$XFD$1</formula1>
@@ -2548,62 +2654,128 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="IeJpSx+ROfPSigOY2Nk0iQkOcv1aUR+7iJV3+Fbsea1dg73v8AT5SOpz8c5mN0mKMauwaefL9wa9i7RT24W/3A==" saltValue="UpwSP/d2uDyu0jnEk+lAEA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -2639,290 +2811,292 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="106" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:1" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="107" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+    <row r="7" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="67" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="108" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="108" t="s">
+    <row r="8" spans="1:1" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="68" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="109" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+    <row r="9" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="110" t="s">
+    <row r="10" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="111" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="111" t="s">
+    <row r="11" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="112" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112" t="s">
+    <row r="12" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="113" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
+    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="114" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="114" t="s">
+    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="115" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="115" t="s">
+    <row r="15" spans="1:1" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="116" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="116" t="s">
+    <row r="16" spans="1:1" s="60" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="69" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="117" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="117" t="s">
+    <row r="17" spans="1:1" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="70" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="118" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="118" t="s">
+    <row r="18" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="119" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="119" t="s">
+    <row r="19" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="120" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="120" t="s">
+    <row r="20" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="121" t="s">
+    <row r="21" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="122" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="122" t="s">
+    <row r="22" spans="1:1" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="123" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="123" t="s">
+    <row r="26" spans="1:1" s="62" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="71" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="124" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="124" t="s">
+    <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="125" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="125" t="s">
+    <row r="28" spans="1:1" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="72" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="126" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="126" t="s">
+    <row r="29" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="127" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="127" t="s">
+    <row r="30" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="128" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="128" t="s">
+    <row r="31" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="129" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="129" t="s">
+    <row r="32" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="130" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="130" t="s">
+    <row r="33" spans="1:1" s="64" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="73" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="131" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="131" t="s">
+    <row r="34" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="132" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="132" t="s">
+    <row r="35" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="133" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="133" t="s">
+    <row r="36" spans="1:1" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="134" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="134" t="s">
+    <row r="37" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:1" s="135" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="135" t="s">
+    <row r="51" spans="1:1" s="65" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="74" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="136" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="136" t="s">
+    <row r="52" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1" s="137" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="137" t="s">
+    <row r="53" spans="1:1" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="C4hM6jw+Jps0ROV/CtoFZSUVwMjSOmuwCxNerG9JcNaXmC8i7iz0PYxkeIBKHzI9z0Syq2R3dE72Rv854PAnpg==" saltValue="whpi3brue2sCzUxgTXmRyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="B38:SG38 B27:SG27 B14:SG15" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>$B$1:$XFD$1</formula1>
@@ -2970,91 +3144,138 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="138" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="138" t="s">
+    <row r="1" spans="1:1" s="75" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="139" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:1" s="76" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="78" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="140" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140" t="s">
+    <row r="11" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="141" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="141" t="s">
+    <row r="12" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>165</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rCgMh9NBzuYtfsAR1fZZ1nzYz9FMBPEPg7x0rlkdFHAVa3TFQJ9A205McT+9/73xqEzfBfHjqGCyrejaF/lpVQ==" saltValue="zP7uUCIlxaf4JaFN1UFZBw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>